<commit_message>
updates with basic visualization.
</commit_message>
<xml_diff>
--- a/Isotope_Data.xlsx
+++ b/Isotope_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenbock/Library/CloudStorage/Box-Box/Hayden's Shared Folder/GitHub/Rochester_Isotope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9519DC63-9FEE-8D4E-BCF4-4F59E8280655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD306D1B-7E5A-1042-8E9D-EECAE6383BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{BBB7FBF7-3033-F044-AE8F-90462D6E2C8A}"/>
   </bookViews>
@@ -413,9 +413,6 @@
     <t>Taxa</t>
   </si>
   <si>
-    <t>∆15N_vs_air</t>
-  </si>
-  <si>
     <t>ATOM%_15N</t>
   </si>
   <si>
@@ -425,9 +422,6 @@
     <t>N_%concentration</t>
   </si>
   <si>
-    <t>∆_13C_vs_IntStandard</t>
-  </si>
-  <si>
     <t>Atom%_13C</t>
   </si>
   <si>
@@ -435,6 +429,12 @@
   </si>
   <si>
     <t>C_%concentration</t>
+  </si>
+  <si>
+    <t>DELTA_15N_vs_air</t>
+  </si>
+  <si>
+    <t>DELTA_13C_vs_IntStandard</t>
   </si>
 </sst>
 </file>
@@ -476,28 +476,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -810,7 +789,7 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,28 +821,28 @@
         <v>124</v>
       </c>
       <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>130</v>
-      </c>
-      <c r="K1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>